<commit_message>
Implemented exclude from automation option
</commit_message>
<xml_diff>
--- a/assets/UB Template.xlsx
+++ b/assets/UB Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C2AD52-2A7B-4320-ADBD-A93DC7D39168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E129708-512F-4B6E-BB5C-FAC94BD20304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -709,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7759B226-B548-469F-A5B2-76DE4BBA961D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -926,9 +926,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>